<commit_message>
add wait visibility to prevent missed collecting data
</commit_message>
<xml_diff>
--- a/food.xlsx
+++ b/food.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,7 +532,11 @@
       <c r="C4" t="n">
         <v>38500</v>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Latte Trà Xanh</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>COFFEE - ESPRESSO</t>
@@ -554,7 +558,11 @@
       <c r="C5" t="n">
         <v>41300</v>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Cà phê Almond Macchiato (Lớp Foam Phô Mai)</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>COFFEE - ESPRESSO</t>
@@ -650,7 +658,11 @@
       <c r="C9" t="n">
         <v>38500</v>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Cà phê Cappuccino</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>COFFEE - ESPRESSO</t>
@@ -672,7 +684,11 @@
       <c r="C10" t="n">
         <v>38500</v>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Cà phê latte</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>COFFEE - ESPRESSO</t>
@@ -688,20 +704,24 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mocha</t>
+          <t>Strawberry &amp; Pink Guava Tea</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>38500</v>
       </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Trà dâu ổi hồng</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>COFFEE - ESPRESSO</t>
+          <t>TEA</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -710,20 +730,24 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Caramel Caffé Macchiato (Cheese Foam)</t>
+          <t>Peach Tea</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>41300</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
+        <v>38500</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Trà Đào</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>COFFEE - ESPRESSO</t>
+          <t>TEA</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -732,7 +756,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Strawberry &amp; Pink Guava Tea</t>
+          <t>Fresh Fruit Tea</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -740,7 +764,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Trà dâu ổi hồng</t>
+          <t>Trà trái cây tươi</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -758,7 +782,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Peach Tea</t>
+          <t>Honey Tea</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -766,7 +790,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Trà Đào</t>
+          <t>Trà mật ong</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -775,7 +799,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -784,7 +808,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Honey Tea</t>
+          <t>Mango Tea</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -792,7 +816,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Trà mật ong</t>
+          <t>Trà Xoài</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -810,7 +834,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Fresh Fruit Tea</t>
+          <t>Oolong Milk Tea</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -818,16 +842,16 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Trà trái cây tươi</t>
+          <t>Trà sữa Oolong</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>TEA</t>
+          <t>MILK TEA</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -836,7 +860,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Mango Tea</t>
+          <t>Roasted Hazelnut Milk Tea</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -844,16 +868,16 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Trà Xoài</t>
+          <t>Trà sữa hạt phỉ</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>TEA</t>
+          <t>MILK TEA</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -862,7 +886,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Oolong Milk Tea</t>
+          <t>Jasmine Milk Tea</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -870,7 +894,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Trà sữa Oolong</t>
+          <t>Trà sữa Lài nguyên lá</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -888,7 +912,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Roasted Hazelnut Milk Tea</t>
+          <t>Earl Grey Milk Tea</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -896,7 +920,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Trà sữa hạt phỉ</t>
+          <t>Trà Sữa Earl Grey</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -914,7 +938,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Jasmine Milk Tea</t>
+          <t>RaspBerry Milk Tea</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -922,7 +946,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Trà sữa Lài nguyên lá</t>
+          <t>Trà sữa dâu rừng</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -940,7 +964,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Earl Grey Milk Tea</t>
+          <t>Black Tea Full Leaf</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -948,7 +972,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Trà Sữa Earl Grey</t>
+          <t>Trà sữa Trà Đen Nguyên Lá</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -957,7 +981,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
@@ -966,7 +990,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>RaspBerry Milk Tea</t>
+          <t>Macchiato with Cheese Foamed</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -974,7 +998,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Trà sữa dâu rừng</t>
+          <t>Trà sữa macchiato</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -983,7 +1007,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
@@ -992,24 +1016,24 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Black Tea Full Leaf</t>
+          <t>Cheesecake Frappé</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>38500</v>
+        <v>41300</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Trà sữa Trà Đen Nguyên Lá</t>
+          <t>Bánh phô mai đá xay</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>MILK TEA</t>
+          <t>BLENDED FRAPPES</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24">
@@ -1018,24 +1042,24 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Macchiato with Cheese Foamed</t>
+          <t>Green Tea Frappé</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>38500</v>
+        <v>41300</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Trà sữa macchiato</t>
+          <t>Trà Xanh Đá Xay</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>MILK TEA</t>
+          <t>BLENDED FRAPPES</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
@@ -1044,7 +1068,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Cheesecake Frappé</t>
+          <t>Tiramisu Cake Frappé</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1052,7 +1076,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Bánh phô mai đá xay</t>
+          <t>Bánh Tiramisu đá xay</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1070,7 +1094,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Green Tea Frappé</t>
+          <t>Double Chocolate Frappé</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1078,7 +1102,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Trà Xanh Đá Xay</t>
+          <t>Sô-cô-la đá xay</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1096,7 +1120,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Tiramisu Cake Frappé</t>
+          <t>Mocha Frappé</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1104,7 +1128,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Bánh Tiramisu đá xay</t>
+          <t>Cà Phê Mocha Đá Xay</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1122,7 +1146,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Double Chocolate Frappé</t>
+          <t>Vanilla Caramel Frappé</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1130,7 +1154,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Sô-cô-la đá xay</t>
+          <t>Vanilla caramel đá xay</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1139,58 +1163,6 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Mocha Frappé</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>41300</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Cà Phê Mocha Đá Xay</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>BLENDED FRAPPES</t>
-        </is>
-      </c>
-      <c r="F29" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Vanilla Caramel Frappé</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>41300</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Vanilla caramel đá xay</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>BLENDED FRAPPES</t>
-        </is>
-      </c>
-      <c r="F30" t="n">
         <v>6</v>
       </c>
     </row>

</xml_diff>